<commit_message>
Update import Khach Hang tu excel
</commit_message>
<xml_diff>
--- a/ReportDocument/SMK/SMK1.xlsx
+++ b/ReportDocument/SMK/SMK1.xlsx
@@ -1,25 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\BlueStarGroup\ReportDocument\SMK\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="7485" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ma hang hoa" sheetId="2" r:id="rId1"/>
-    <sheet name="KTFORMAT" sheetId="1" state="hidden" r:id="rId2"/>
-    <sheet name="Ma khach hang" sheetId="3" r:id="rId3"/>
+    <sheet name="LoaiHangHoa" sheetId="5" r:id="rId2"/>
+    <sheet name="KTFORMAT" sheetId="1" state="hidden" r:id="rId3"/>
+    <sheet name="Ma khach hang" sheetId="3" r:id="rId4"/>
+    <sheet name="DVT" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ma hang hoa'!$A$4:$F$195</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="835">
   <si>
     <t>Tổng</t>
   </si>
@@ -2449,13 +2456,88 @@
   </si>
   <si>
     <t>0107749754</t>
+  </si>
+  <si>
+    <t>LIT</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>KET</t>
+  </si>
+  <si>
+    <t>LON</t>
+  </si>
+  <si>
+    <t>HOP</t>
+  </si>
+  <si>
+    <t>THUNG</t>
+  </si>
+  <si>
+    <t>CHAI</t>
+  </si>
+  <si>
+    <t>TUI</t>
+  </si>
+  <si>
+    <t>XO</t>
+  </si>
+  <si>
+    <t>BINH</t>
+  </si>
+  <si>
+    <t>PHUY</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>CAI</t>
+  </si>
+  <si>
+    <t>COC</t>
+  </si>
+  <si>
+    <t>BICH</t>
+  </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>GOI</t>
+  </si>
+  <si>
+    <t>BO</t>
+  </si>
+  <si>
+    <t>CHIEC</t>
+  </si>
+  <si>
+    <t>Mã ĐVT</t>
+  </si>
+  <si>
+    <t>Tên ĐVT</t>
+  </si>
+  <si>
+    <t>KHAC</t>
+  </si>
+  <si>
+    <t>Mã Loại SP</t>
+  </si>
+  <si>
+    <t>Tên Loại SP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2590,6 +2672,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2637,7 +2722,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2672,7 +2757,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2883,11 +2968,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F195"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D194"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -2898,12 +2983,12 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="8" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18.75">
       <c r="A2" s="7" t="s">
         <v>420</v>
       </c>
@@ -2913,7 +2998,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>413</v>
       </c>
@@ -2933,7 +3018,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -2943,8 +3028,8 @@
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>4</v>
+      <c r="D5" s="12" t="s">
+        <v>832</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>4</v>
@@ -2953,7 +3038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
@@ -2963,8 +3048,8 @@
       <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>4</v>
+      <c r="D6" s="12" t="s">
+        <v>832</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>4</v>
@@ -2973,7 +3058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -2993,7 +3078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -3013,7 +3098,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -3033,7 +3118,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -3053,7 +3138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -3073,7 +3158,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
@@ -3093,7 +3178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
@@ -3113,7 +3198,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
@@ -3133,7 +3218,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
@@ -3153,7 +3238,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
@@ -3173,7 +3258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
@@ -3193,7 +3278,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="5" t="s">
         <v>8</v>
       </c>
@@ -3213,7 +3298,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
@@ -3233,7 +3318,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="5" t="s">
         <v>8</v>
       </c>
@@ -3253,7 +3338,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
@@ -3273,7 +3358,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -3293,7 +3378,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="5" t="s">
         <v>8</v>
       </c>
@@ -3313,7 +3398,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -3333,7 +3418,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="5" t="s">
         <v>8</v>
       </c>
@@ -3353,7 +3438,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="5" t="s">
         <v>8</v>
       </c>
@@ -3373,7 +3458,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
@@ -3393,7 +3478,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="5" t="s">
         <v>8</v>
       </c>
@@ -3413,7 +3498,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="5" t="s">
         <v>8</v>
       </c>
@@ -3433,7 +3518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="5" t="s">
         <v>8</v>
       </c>
@@ -3453,7 +3538,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="5" t="s">
         <v>8</v>
       </c>
@@ -3473,7 +3558,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
@@ -3493,7 +3578,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="5" t="s">
         <v>8</v>
       </c>
@@ -3513,7 +3598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="5" t="s">
         <v>8</v>
       </c>
@@ -3533,7 +3618,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="5" t="s">
         <v>8</v>
       </c>
@@ -3553,7 +3638,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="5" t="s">
         <v>8</v>
       </c>
@@ -3573,7 +3658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="5" t="s">
         <v>8</v>
       </c>
@@ -3593,7 +3678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="5" t="s">
         <v>8</v>
       </c>
@@ -3613,7 +3698,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="5" t="s">
         <v>8</v>
       </c>
@@ -3633,7 +3718,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="5" t="s">
         <v>8</v>
       </c>
@@ -3653,7 +3738,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="5" t="s">
         <v>8</v>
       </c>
@@ -3673,7 +3758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="5" t="s">
         <v>8</v>
       </c>
@@ -3693,7 +3778,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="5" t="s">
         <v>8</v>
       </c>
@@ -3713,7 +3798,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="5" t="s">
         <v>8</v>
       </c>
@@ -3733,7 +3818,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="5" t="s">
         <v>8</v>
       </c>
@@ -3753,7 +3838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="5" t="s">
         <v>8</v>
       </c>
@@ -3773,7 +3858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="5" t="s">
         <v>8</v>
       </c>
@@ -3793,7 +3878,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="5" t="s">
         <v>8</v>
       </c>
@@ -3813,7 +3898,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="5" t="s">
         <v>8</v>
       </c>
@@ -3833,7 +3918,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="5" t="s">
         <v>8</v>
       </c>
@@ -3853,7 +3938,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="5" t="s">
         <v>8</v>
       </c>
@@ -3873,7 +3958,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="5" t="s">
         <v>8</v>
       </c>
@@ -3893,7 +3978,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="5" t="s">
         <v>8</v>
       </c>
@@ -3913,7 +3998,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="5" t="s">
         <v>8</v>
       </c>
@@ -3933,7 +4018,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="5" t="s">
         <v>8</v>
       </c>
@@ -3953,7 +4038,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="5" t="s">
         <v>8</v>
       </c>
@@ -3973,7 +4058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="5" t="s">
         <v>8</v>
       </c>
@@ -3993,7 +4078,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="5" t="s">
         <v>8</v>
       </c>
@@ -4013,7 +4098,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="5" t="s">
         <v>8</v>
       </c>
@@ -4033,7 +4118,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="5" t="s">
         <v>8</v>
       </c>
@@ -4053,7 +4138,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="5" t="s">
         <v>8</v>
       </c>
@@ -4073,7 +4158,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="5" t="s">
         <v>8</v>
       </c>
@@ -4093,7 +4178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="5" t="s">
         <v>8</v>
       </c>
@@ -4113,7 +4198,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="5" t="s">
         <v>8</v>
       </c>
@@ -4133,7 +4218,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" s="5" t="s">
         <v>8</v>
       </c>
@@ -4153,7 +4238,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" s="5" t="s">
         <v>8</v>
       </c>
@@ -4173,7 +4258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" s="5" t="s">
         <v>8</v>
       </c>
@@ -4193,7 +4278,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" s="5" t="s">
         <v>8</v>
       </c>
@@ -4213,7 +4298,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" s="5" t="s">
         <v>8</v>
       </c>
@@ -4233,7 +4318,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" s="5" t="s">
         <v>8</v>
       </c>
@@ -4253,7 +4338,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" s="5" t="s">
         <v>8</v>
       </c>
@@ -4273,7 +4358,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" s="5" t="s">
         <v>8</v>
       </c>
@@ -4293,7 +4378,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73" s="5" t="s">
         <v>8</v>
       </c>
@@ -4313,7 +4398,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" s="5" t="s">
         <v>8</v>
       </c>
@@ -4333,7 +4418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75" s="5" t="s">
         <v>8</v>
       </c>
@@ -4353,7 +4438,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76" s="5" t="s">
         <v>8</v>
       </c>
@@ -4373,7 +4458,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77" s="5" t="s">
         <v>8</v>
       </c>
@@ -4393,7 +4478,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78" s="5" t="s">
         <v>8</v>
       </c>
@@ -4413,7 +4498,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" s="5" t="s">
         <v>8</v>
       </c>
@@ -4433,7 +4518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" s="5" t="s">
         <v>8</v>
       </c>
@@ -4453,7 +4538,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81" s="5" t="s">
         <v>8</v>
       </c>
@@ -4473,7 +4558,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82" s="5" t="s">
         <v>8</v>
       </c>
@@ -4493,7 +4578,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83" s="5" t="s">
         <v>8</v>
       </c>
@@ -4513,7 +4598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84" s="5" t="s">
         <v>8</v>
       </c>
@@ -4533,7 +4618,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" s="5" t="s">
         <v>8</v>
       </c>
@@ -4553,7 +4638,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86" s="5" t="s">
         <v>8</v>
       </c>
@@ -4573,7 +4658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="5" t="s">
         <v>8</v>
       </c>
@@ -4593,7 +4678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="5" t="s">
         <v>8</v>
       </c>
@@ -4613,7 +4698,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="5" t="s">
         <v>8</v>
       </c>
@@ -4633,7 +4718,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="5" t="s">
         <v>8</v>
       </c>
@@ -4653,7 +4738,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="5" t="s">
         <v>8</v>
       </c>
@@ -4673,7 +4758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" s="5" t="s">
         <v>8</v>
       </c>
@@ -4693,7 +4778,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93" s="5" t="s">
         <v>8</v>
       </c>
@@ -4713,7 +4798,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="5" t="s">
         <v>8</v>
       </c>
@@ -4733,7 +4818,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" s="5" t="s">
         <v>8</v>
       </c>
@@ -4753,7 +4838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" s="5" t="s">
         <v>8</v>
       </c>
@@ -4773,7 +4858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97" s="5" t="s">
         <v>8</v>
       </c>
@@ -4793,7 +4878,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="A98" s="5" t="s">
         <v>8</v>
       </c>
@@ -4813,7 +4898,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99" s="5" t="s">
         <v>8</v>
       </c>
@@ -4833,7 +4918,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100" s="5" t="s">
         <v>8</v>
       </c>
@@ -4853,7 +4938,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="A101" s="5" t="s">
         <v>8</v>
       </c>
@@ -4873,7 +4958,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6">
       <c r="A102" s="5" t="s">
         <v>8</v>
       </c>
@@ -4893,7 +4978,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6">
       <c r="A103" s="5" t="s">
         <v>8</v>
       </c>
@@ -4913,7 +4998,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6">
       <c r="A104" s="5" t="s">
         <v>8</v>
       </c>
@@ -4933,7 +5018,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6">
       <c r="A105" s="5" t="s">
         <v>8</v>
       </c>
@@ -4953,7 +5038,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6">
       <c r="A106" s="5" t="s">
         <v>8</v>
       </c>
@@ -4973,7 +5058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6">
       <c r="A107" s="5" t="s">
         <v>8</v>
       </c>
@@ -4993,7 +5078,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6">
       <c r="A108" s="5" t="s">
         <v>8</v>
       </c>
@@ -5013,7 +5098,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6">
       <c r="A109" s="5" t="s">
         <v>8</v>
       </c>
@@ -5033,7 +5118,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6">
       <c r="A110" s="5" t="s">
         <v>8</v>
       </c>
@@ -5053,7 +5138,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6">
       <c r="A111" s="5" t="s">
         <v>8</v>
       </c>
@@ -5073,7 +5158,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6">
       <c r="A112" s="5" t="s">
         <v>8</v>
       </c>
@@ -5093,7 +5178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6">
       <c r="A113" s="5" t="s">
         <v>8</v>
       </c>
@@ -5113,7 +5198,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6">
       <c r="A114" s="5" t="s">
         <v>8</v>
       </c>
@@ -5133,7 +5218,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6">
       <c r="A115" s="5" t="s">
         <v>8</v>
       </c>
@@ -5153,7 +5238,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6">
       <c r="A116" s="5" t="s">
         <v>8</v>
       </c>
@@ -5173,7 +5258,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6">
       <c r="A117" s="5" t="s">
         <v>8</v>
       </c>
@@ -5193,7 +5278,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6">
       <c r="A118" s="5" t="s">
         <v>8</v>
       </c>
@@ -5213,7 +5298,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6">
       <c r="A119" s="5" t="s">
         <v>8</v>
       </c>
@@ -5233,7 +5318,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6">
       <c r="A120" s="5" t="s">
         <v>8</v>
       </c>
@@ -5253,7 +5338,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6">
       <c r="A121" s="5" t="s">
         <v>8</v>
       </c>
@@ -5273,7 +5358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6">
       <c r="A122" s="5" t="s">
         <v>8</v>
       </c>
@@ -5293,7 +5378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6">
       <c r="A123" s="5" t="s">
         <v>8</v>
       </c>
@@ -5313,7 +5398,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6">
       <c r="A124" s="5" t="s">
         <v>8</v>
       </c>
@@ -5333,7 +5418,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6">
       <c r="A125" s="5" t="s">
         <v>8</v>
       </c>
@@ -5353,7 +5438,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6">
       <c r="A126" s="5" t="s">
         <v>8</v>
       </c>
@@ -5373,7 +5458,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6">
       <c r="A127" s="5" t="s">
         <v>8</v>
       </c>
@@ -5383,8 +5468,8 @@
       <c r="C127" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="D127" s="5" t="s">
-        <v>4</v>
+      <c r="D127" s="12" t="s">
+        <v>832</v>
       </c>
       <c r="E127" s="5" t="s">
         <v>4</v>
@@ -5393,7 +5478,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6">
       <c r="A128" s="5" t="s">
         <v>8</v>
       </c>
@@ -5413,7 +5498,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6">
       <c r="A129" s="5" t="s">
         <v>8</v>
       </c>
@@ -5433,7 +5518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6">
       <c r="A130" s="5" t="s">
         <v>8</v>
       </c>
@@ -5453,7 +5538,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6">
       <c r="A131" s="5" t="s">
         <v>8</v>
       </c>
@@ -5473,7 +5558,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6">
       <c r="A132" s="5" t="s">
         <v>8</v>
       </c>
@@ -5493,7 +5578,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6">
       <c r="A133" s="5" t="s">
         <v>8</v>
       </c>
@@ -5513,7 +5598,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6">
       <c r="A134" s="5" t="s">
         <v>8</v>
       </c>
@@ -5533,7 +5618,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6">
       <c r="A135" s="5" t="s">
         <v>8</v>
       </c>
@@ -5553,7 +5638,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6">
       <c r="A136" s="5" t="s">
         <v>8</v>
       </c>
@@ -5573,7 +5658,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6">
       <c r="A137" s="5" t="s">
         <v>8</v>
       </c>
@@ -5593,7 +5678,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6">
       <c r="A138" s="5" t="s">
         <v>8</v>
       </c>
@@ -5613,7 +5698,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6">
       <c r="A139" s="5" t="s">
         <v>8</v>
       </c>
@@ -5633,7 +5718,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6">
       <c r="A140" s="5" t="s">
         <v>8</v>
       </c>
@@ -5653,7 +5738,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6">
       <c r="A141" s="5" t="s">
         <v>8</v>
       </c>
@@ -5673,7 +5758,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6">
       <c r="A142" s="5" t="s">
         <v>8</v>
       </c>
@@ -5693,7 +5778,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6">
       <c r="A143" s="5" t="s">
         <v>8</v>
       </c>
@@ -5713,7 +5798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6">
       <c r="A144" s="5" t="s">
         <v>8</v>
       </c>
@@ -5733,7 +5818,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6">
       <c r="A145" s="5" t="s">
         <v>8</v>
       </c>
@@ -5753,7 +5838,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6">
       <c r="A146" s="5" t="s">
         <v>8</v>
       </c>
@@ -5763,8 +5848,8 @@
       <c r="C146" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="D146" s="5" t="s">
-        <v>4</v>
+      <c r="D146" s="12" t="s">
+        <v>832</v>
       </c>
       <c r="E146" s="5" t="s">
         <v>4</v>
@@ -5773,7 +5858,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6">
       <c r="A147" s="5" t="s">
         <v>8</v>
       </c>
@@ -5783,8 +5868,8 @@
       <c r="C147" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="D147" s="5" t="s">
-        <v>4</v>
+      <c r="D147" s="12" t="s">
+        <v>832</v>
       </c>
       <c r="E147" s="5" t="s">
         <v>4</v>
@@ -5793,7 +5878,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6">
       <c r="A148" s="5" t="s">
         <v>8</v>
       </c>
@@ -5803,8 +5888,8 @@
       <c r="C148" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="D148" s="5" t="s">
-        <v>4</v>
+      <c r="D148" s="12" t="s">
+        <v>832</v>
       </c>
       <c r="E148" s="5" t="s">
         <v>4</v>
@@ -5813,7 +5898,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6">
       <c r="A149" s="5" t="s">
         <v>8</v>
       </c>
@@ -5833,7 +5918,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6">
       <c r="A150" s="5" t="s">
         <v>8</v>
       </c>
@@ -5853,7 +5938,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6">
       <c r="A151" s="5" t="s">
         <v>8</v>
       </c>
@@ -5873,7 +5958,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6">
       <c r="A152" s="5" t="s">
         <v>8</v>
       </c>
@@ -5893,7 +5978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6">
       <c r="A153" s="5" t="s">
         <v>8</v>
       </c>
@@ -5913,7 +5998,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6">
       <c r="A154" s="5" t="s">
         <v>8</v>
       </c>
@@ -5933,7 +6018,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6">
       <c r="A155" s="5" t="s">
         <v>8</v>
       </c>
@@ -5953,7 +6038,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6">
       <c r="A156" s="5" t="s">
         <v>8</v>
       </c>
@@ -5973,7 +6058,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6">
       <c r="A157" s="5" t="s">
         <v>8</v>
       </c>
@@ -5993,7 +6078,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6">
       <c r="A158" s="5" t="s">
         <v>8</v>
       </c>
@@ -6013,7 +6098,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6">
       <c r="A159" s="5" t="s">
         <v>8</v>
       </c>
@@ -6033,7 +6118,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6">
       <c r="A160" s="5" t="s">
         <v>8</v>
       </c>
@@ -6053,7 +6138,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6">
       <c r="A161" s="5" t="s">
         <v>8</v>
       </c>
@@ -6073,7 +6158,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6">
       <c r="A162" s="5" t="s">
         <v>8</v>
       </c>
@@ -6093,7 +6178,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6">
       <c r="A163" s="5" t="s">
         <v>8</v>
       </c>
@@ -6113,7 +6198,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6">
       <c r="A164" s="5" t="s">
         <v>8</v>
       </c>
@@ -6133,7 +6218,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6">
       <c r="A165" s="5" t="s">
         <v>8</v>
       </c>
@@ -6153,7 +6238,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6">
       <c r="A166" s="5" t="s">
         <v>8</v>
       </c>
@@ -6173,7 +6258,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6">
       <c r="A167" s="5" t="s">
         <v>8</v>
       </c>
@@ -6193,7 +6278,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6">
       <c r="A168" s="5" t="s">
         <v>8</v>
       </c>
@@ -6213,7 +6298,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6">
       <c r="A169" s="5" t="s">
         <v>8</v>
       </c>
@@ -6233,7 +6318,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6">
       <c r="A170" s="5" t="s">
         <v>8</v>
       </c>
@@ -6253,7 +6338,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6">
       <c r="A171" s="5" t="s">
         <v>8</v>
       </c>
@@ -6273,7 +6358,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6">
       <c r="A172" s="5" t="s">
         <v>8</v>
       </c>
@@ -6293,7 +6378,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6">
       <c r="A173" s="5" t="s">
         <v>8</v>
       </c>
@@ -6313,7 +6398,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6">
       <c r="A174" s="5" t="s">
         <v>8</v>
       </c>
@@ -6333,7 +6418,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6">
       <c r="A175" s="5" t="s">
         <v>8</v>
       </c>
@@ -6353,7 +6438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6">
       <c r="A176" s="5" t="s">
         <v>8</v>
       </c>
@@ -6373,7 +6458,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6">
       <c r="A177" s="5" t="s">
         <v>8</v>
       </c>
@@ -6393,7 +6478,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6">
       <c r="A178" s="5" t="s">
         <v>8</v>
       </c>
@@ -6413,7 +6498,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6">
       <c r="A179" s="5" t="s">
         <v>8</v>
       </c>
@@ -6433,7 +6518,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6">
       <c r="A180" s="5" t="s">
         <v>8</v>
       </c>
@@ -6453,7 +6538,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6">
       <c r="A181" s="5" t="s">
         <v>8</v>
       </c>
@@ -6473,7 +6558,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6">
       <c r="A182" s="5" t="s">
         <v>8</v>
       </c>
@@ -6493,7 +6578,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6">
       <c r="A183" s="5" t="s">
         <v>8</v>
       </c>
@@ -6513,7 +6598,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6">
       <c r="A184" s="5" t="s">
         <v>8</v>
       </c>
@@ -6533,7 +6618,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6">
       <c r="A185" s="5" t="s">
         <v>8</v>
       </c>
@@ -6553,7 +6638,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6">
       <c r="A186" s="5" t="s">
         <v>8</v>
       </c>
@@ -6573,7 +6658,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6">
       <c r="A187" s="5" t="s">
         <v>8</v>
       </c>
@@ -6593,7 +6678,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6">
       <c r="A188" s="5" t="s">
         <v>8</v>
       </c>
@@ -6613,7 +6698,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6">
       <c r="A189" s="5" t="s">
         <v>8</v>
       </c>
@@ -6633,7 +6718,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6">
       <c r="A190" s="5" t="s">
         <v>8</v>
       </c>
@@ -6653,7 +6738,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6">
       <c r="A191" s="5" t="s">
         <v>402</v>
       </c>
@@ -6673,7 +6758,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6">
       <c r="A192" s="5" t="s">
         <v>402</v>
       </c>
@@ -6693,7 +6778,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6">
       <c r="A193" s="5" t="s">
         <v>402</v>
       </c>
@@ -6713,7 +6798,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6">
       <c r="A194" s="5" t="s">
         <v>402</v>
       </c>
@@ -6724,7 +6809,7 @@
         <v>411</v>
       </c>
       <c r="D194" s="5" t="s">
-        <v>4</v>
+        <v>832</v>
       </c>
       <c r="E194" s="5" t="s">
         <v>4</v>
@@ -6733,7 +6818,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6">
       <c r="A195" s="4" t="s">
         <v>0</v>
       </c>
@@ -6752,24 +6837,130 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="9" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>833</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="12" t="s">
+        <v>832</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>299</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="2"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="3"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="4"/>
     </row>
   </sheetData>
@@ -6778,22 +6969,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="127.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="101.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="15" t="s">
         <v>419</v>
       </c>
@@ -6803,7 +6994,7 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18.75">
       <c r="A2" s="14" t="s">
         <v>421</v>
       </c>
@@ -6813,7 +7004,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="10" t="s">
         <v>422</v>
       </c>
@@ -6833,7 +7024,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="12" t="s">
         <v>428</v>
       </c>
@@ -6853,7 +7044,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="12" t="s">
         <v>431</v>
       </c>
@@ -6873,7 +7064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="12" t="s">
         <v>433</v>
       </c>
@@ -6893,7 +7084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="12" t="s">
         <v>435</v>
       </c>
@@ -6913,7 +7104,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="12" t="s">
         <v>438</v>
       </c>
@@ -6933,7 +7124,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="12" t="s">
         <v>441</v>
       </c>
@@ -6953,7 +7144,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="12" t="s">
         <v>445</v>
       </c>
@@ -6973,7 +7164,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="12" t="s">
         <v>449</v>
       </c>
@@ -6993,7 +7184,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="12" t="s">
         <v>453</v>
       </c>
@@ -7013,7 +7204,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="12" t="s">
         <v>456</v>
       </c>
@@ -7033,7 +7224,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="12" t="s">
         <v>460</v>
       </c>
@@ -7053,7 +7244,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="12" t="s">
         <v>463</v>
       </c>
@@ -7073,7 +7264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="12" t="s">
         <v>465</v>
       </c>
@@ -7093,7 +7284,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="12" t="s">
         <v>468</v>
       </c>
@@ -7113,7 +7304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="12" t="s">
         <v>470</v>
       </c>
@@ -7133,7 +7324,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="12" t="s">
         <v>474</v>
       </c>
@@ -7153,7 +7344,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="12" t="s">
         <v>478</v>
       </c>
@@ -7173,7 +7364,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="12" t="s">
         <v>482</v>
       </c>
@@ -7193,7 +7384,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="12" t="s">
         <v>486</v>
       </c>
@@ -7213,7 +7404,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="12" t="s">
         <v>17</v>
       </c>
@@ -7233,7 +7424,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="12" t="s">
         <v>493</v>
       </c>
@@ -7253,7 +7444,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="12" t="s">
         <v>496</v>
       </c>
@@ -7273,7 +7464,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="12" t="s">
         <v>500</v>
       </c>
@@ -7293,7 +7484,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="12" t="s">
         <v>504</v>
       </c>
@@ -7313,7 +7504,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="12" t="s">
         <v>508</v>
       </c>
@@ -7333,7 +7524,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="12" t="s">
         <v>512</v>
       </c>
@@ -7353,7 +7544,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="12" t="s">
         <v>516</v>
       </c>
@@ -7373,7 +7564,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="12" t="s">
         <v>520</v>
       </c>
@@ -7393,7 +7584,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="12" t="s">
         <v>524</v>
       </c>
@@ -7413,7 +7604,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="12" t="s">
         <v>528</v>
       </c>
@@ -7433,7 +7624,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="12" t="s">
         <v>532</v>
       </c>
@@ -7453,7 +7644,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="12" t="s">
         <v>536</v>
       </c>
@@ -7473,7 +7664,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="12" t="s">
         <v>540</v>
       </c>
@@ -7493,7 +7684,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="12" t="s">
         <v>544</v>
       </c>
@@ -7513,7 +7704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="12" t="s">
         <v>546</v>
       </c>
@@ -7533,7 +7724,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="12" t="s">
         <v>550</v>
       </c>
@@ -7553,7 +7744,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="12" t="s">
         <v>554</v>
       </c>
@@ -7573,7 +7764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="12" t="s">
         <v>556</v>
       </c>
@@ -7593,7 +7784,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="12" t="s">
         <v>560</v>
       </c>
@@ -7613,7 +7804,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="12" t="s">
         <v>564</v>
       </c>
@@ -7633,7 +7824,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="12" t="s">
         <v>568</v>
       </c>
@@ -7653,7 +7844,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="12" t="s">
         <v>572</v>
       </c>
@@ -7673,7 +7864,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="12" t="s">
         <v>574</v>
       </c>
@@ -7693,7 +7884,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="12" t="s">
         <v>575</v>
       </c>
@@ -7713,7 +7904,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="12" t="s">
         <v>579</v>
       </c>
@@ -7733,7 +7924,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="12" t="s">
         <v>583</v>
       </c>
@@ -7753,7 +7944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="12" t="s">
         <v>585</v>
       </c>
@@ -7773,7 +7964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="12" t="s">
         <v>587</v>
       </c>
@@ -7793,7 +7984,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="12" t="s">
         <v>591</v>
       </c>
@@ -7813,7 +8004,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="12" t="s">
         <v>595</v>
       </c>
@@ -7833,7 +8024,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="12" t="s">
         <v>599</v>
       </c>
@@ -7853,7 +8044,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="12" t="s">
         <v>602</v>
       </c>
@@ -7873,7 +8064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="12" t="s">
         <v>604</v>
       </c>
@@ -7893,7 +8084,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="12" t="s">
         <v>608</v>
       </c>
@@ -7913,7 +8104,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="12" t="s">
         <v>612</v>
       </c>
@@ -7933,7 +8124,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="12" t="s">
         <v>616</v>
       </c>
@@ -7953,7 +8144,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="12" t="s">
         <v>620</v>
       </c>
@@ -7973,7 +8164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="12" t="s">
         <v>623</v>
       </c>
@@ -7993,7 +8184,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="12" t="s">
         <v>624</v>
       </c>
@@ -8013,7 +8204,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="12" t="s">
         <v>628</v>
       </c>
@@ -8033,7 +8224,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" s="12" t="s">
         <v>632</v>
       </c>
@@ -8053,7 +8244,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" s="12" t="s">
         <v>636</v>
       </c>
@@ -8073,7 +8264,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" s="12" t="s">
         <v>640</v>
       </c>
@@ -8093,7 +8284,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" s="12" t="s">
         <v>644</v>
       </c>
@@ -8113,7 +8304,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" s="12" t="s">
         <v>648</v>
       </c>
@@ -8133,7 +8324,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" s="12" t="s">
         <v>652</v>
       </c>
@@ -8153,7 +8344,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" s="12" t="s">
         <v>656</v>
       </c>
@@ -8173,7 +8364,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" s="12" t="s">
         <v>660</v>
       </c>
@@ -8193,7 +8384,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73" s="12" t="s">
         <v>662</v>
       </c>
@@ -8213,7 +8404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" s="12" t="s">
         <v>665</v>
       </c>
@@ -8233,7 +8424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75" s="12" t="s">
         <v>668</v>
       </c>
@@ -8253,7 +8444,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76" s="12" t="s">
         <v>670</v>
       </c>
@@ -8273,7 +8464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77" s="12" t="s">
         <v>672</v>
       </c>
@@ -8293,7 +8484,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78" s="12" t="s">
         <v>675</v>
       </c>
@@ -8313,7 +8504,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" s="12" t="s">
         <v>679</v>
       </c>
@@ -8333,7 +8524,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" s="12" t="s">
         <v>683</v>
       </c>
@@ -8353,7 +8544,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81" s="12" t="s">
         <v>687</v>
       </c>
@@ -8373,7 +8564,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82" s="12" t="s">
         <v>691</v>
       </c>
@@ -8393,7 +8584,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83" s="12" t="s">
         <v>695</v>
       </c>
@@ -8413,7 +8604,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84" s="12" t="s">
         <v>699</v>
       </c>
@@ -8433,7 +8624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" s="12" t="s">
         <v>701</v>
       </c>
@@ -8453,7 +8644,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86" s="12" t="s">
         <v>705</v>
       </c>
@@ -8473,7 +8664,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="12" t="s">
         <v>709</v>
       </c>
@@ -8493,7 +8684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="12" t="s">
         <v>711</v>
       </c>
@@ -8513,7 +8704,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="12" t="s">
         <v>715</v>
       </c>
@@ -8533,7 +8724,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="12" t="s">
         <v>719</v>
       </c>
@@ -8553,7 +8744,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="12" t="s">
         <v>723</v>
       </c>
@@ -8573,7 +8764,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" s="12" t="s">
         <v>727</v>
       </c>
@@ -8593,7 +8784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93" s="12" t="s">
         <v>729</v>
       </c>
@@ -8613,7 +8804,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="12" t="s">
         <v>733</v>
       </c>
@@ -8633,7 +8824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" s="12" t="s">
         <v>735</v>
       </c>
@@ -8653,7 +8844,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" s="12" t="s">
         <v>739</v>
       </c>
@@ -8673,7 +8864,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97" s="12" t="s">
         <v>743</v>
       </c>
@@ -8693,7 +8884,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="A98" s="12" t="s">
         <v>747</v>
       </c>
@@ -8713,7 +8904,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99" s="12" t="s">
         <v>750</v>
       </c>
@@ -8733,7 +8924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100" s="12" t="s">
         <v>752</v>
       </c>
@@ -8753,7 +8944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="A101" s="12" t="s">
         <v>754</v>
       </c>
@@ -8773,7 +8964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6">
       <c r="A102" s="12" t="s">
         <v>756</v>
       </c>
@@ -8793,7 +8984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6">
       <c r="A103" s="12" t="s">
         <v>759</v>
       </c>
@@ -8813,7 +9004,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6">
       <c r="A104" s="12" t="s">
         <v>762</v>
       </c>
@@ -8833,7 +9024,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6">
       <c r="A105" s="12" t="s">
         <v>766</v>
       </c>
@@ -8853,7 +9044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6">
       <c r="A106" s="12" t="s">
         <v>768</v>
       </c>
@@ -8873,7 +9064,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6">
       <c r="A107" s="12" t="s">
         <v>772</v>
       </c>
@@ -8893,7 +9084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6">
       <c r="A108" s="12" t="s">
         <v>774</v>
       </c>
@@ -8913,7 +9104,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6">
       <c r="A109" s="12" t="s">
         <v>778</v>
       </c>
@@ -8933,7 +9124,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6">
       <c r="A110" s="12" t="s">
         <v>782</v>
       </c>
@@ -8953,7 +9144,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6">
       <c r="A111" s="12" t="s">
         <v>786</v>
       </c>
@@ -8973,7 +9164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6">
       <c r="A112" s="12" t="s">
         <v>788</v>
       </c>
@@ -8993,7 +9184,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6">
       <c r="A113" s="12" t="s">
         <v>792</v>
       </c>
@@ -9013,7 +9204,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6">
       <c r="A114" s="12" t="s">
         <v>796</v>
       </c>
@@ -9033,7 +9224,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6">
       <c r="A115" s="12" t="s">
         <v>799</v>
       </c>
@@ -9053,7 +9244,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6">
       <c r="A116" s="12" t="s">
         <v>803</v>
       </c>
@@ -9073,7 +9264,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6">
       <c r="A117" s="12" t="s">
         <v>294</v>
       </c>
@@ -9093,7 +9284,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6">
       <c r="A118" s="11" t="s">
         <v>0</v>
       </c>
@@ -9106,4 +9297,196 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="9" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>830</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="9" t="s">
+        <v>824</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="9" t="s">
+        <v>819</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="9" t="s">
+        <v>828</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="9" t="s">
+        <v>822</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="9" t="s">
+        <v>829</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="9" t="s">
+        <v>823</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="9" t="s">
+        <v>825</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="9" t="s">
+        <v>827</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="9" t="s">
+        <v>814</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="9" t="s">
+        <v>812</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="9" t="s">
+        <v>810</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="9" t="s">
+        <v>811</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="9" t="s">
+        <v>813</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="9" t="s">
+        <v>820</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="9" t="s">
+        <v>815</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="9" t="s">
+        <v>817</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="9" t="s">
+        <v>821</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="9" t="s">
+        <v>818</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:B190">
+    <sortCondition ref="B1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>